<commit_message>
Pivoted to Pandoc in a big way
</commit_message>
<xml_diff>
--- a/reqs.xlsx
+++ b/reqs.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$14</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$13</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,13 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
-  <si>
-    <t xml:space="preserve">section</t>
-  </si>
-  <si>
-    <t xml:space="preserve">style</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -43,31 +37,19 @@
     <t xml:space="preserve">trace</t>
   </si>
   <si>
-    <t xml:space="preserve">title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Computer Requirements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">heading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">para</t>
+    <t xml:space="preserve"># Scope</t>
   </si>
   <si>
     <t xml:space="preserve">This document includes an example of writing requirements via a spreadsheet. I have very mixed feelings about this.</t>
   </si>
   <si>
-    <t xml:space="preserve">References</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Form Factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dimensions</t>
+    <t xml:space="preserve"># References</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Form Factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## Dimensions</t>
   </si>
   <si>
     <t xml:space="preserve">The computer shall be no larger than 4x5x6.</t>
@@ -85,7 +67,7 @@
     <t xml:space="preserve">crd-5</t>
   </si>
   <si>
-    <t xml:space="preserve">Appearance</t>
+    <t xml:space="preserve">## Appearance</t>
   </si>
   <si>
     <t xml:space="preserve">The computer shall be green or blue.</t>
@@ -94,10 +76,10 @@
     <t xml:space="preserve">crd-12</t>
   </si>
   <si>
-    <t xml:space="preserve">Smells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the current date is a Thursday or Friday, the computer shall smell like apircots.</t>
+    <t xml:space="preserve">## Smells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the current date is a Thursday or Friday, the computer shall smell like apricots.</t>
   </si>
   <si>
     <t xml:space="preserve">crd-1, crd-2</t>
@@ -107,6 +89,49 @@
   </si>
   <si>
     <t xml:space="preserve">crd-773</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Formatting Tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This section checks some Pandoc markdown features.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## Equations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cost of the test cases $c_t$ shall be 15.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This shall be $\alpha = \frac{1-x^2}{\beta - \gamma}$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## Tables</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">This requirement shall have a table.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="FreeMono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Input  Output
+------ -------
+1      10
+2      15.7
+3      17</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -116,7 +141,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -143,6 +168,18 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="FreeMono"/>
+      <family val="3"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -188,7 +225,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -201,6 +238,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,6 +251,30 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+        <sz val="18"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+        <sz val="12"/>
+      </font>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -222,18 +287,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:AMJ20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="76.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -249,22 +313,12 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -272,171 +326,146 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>1</v>
-      </c>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>3</v>
-      </c>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>3.1</v>
+        <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>3.2</v>
+        <v>4</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>3.3</v>
+        <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D13" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="2" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D14" s="2" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="2" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
         <v>27</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F14"/>
+  <autoFilter ref="A1:D13"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="beginsWith" priority="2" operator="beginsWith" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="# " dxfId="0">
+      <formula>LEFT(B1,LEN("# "))="# "</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="3" operator="beginsWith" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="## " dxfId="1">
+      <formula>LEFT(B1,LEN("## "))="## "</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>